<commit_message>
added comments to Q1 code
</commit_message>
<xml_diff>
--- a/Part4Plot.xlsx
+++ b/Part4Plot.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\ECSE 420\HW\HW1\Assignment1_SourceCodes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{845290E4-359F-4417-B397-E4255F8B278E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE8EB042-96EA-4441-9B28-D7484B0A10F5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Part4" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -609,6 +609,14 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.21831233595800525"/>
+          <c:y val="3.2407407407407406E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1938,7 +1946,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">

</xml_diff>